<commit_message>
Browser changes and Linux driver added
</commit_message>
<xml_diff>
--- a/inputFiles/Admin_Login.xlsx
+++ b/inputFiles/Admin_Login.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\eclipse-workspace\EzScheduler\inputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\EzScheduler\EzScheduler\inputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF22AA90-954B-4288-9493-D2D042E8001B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9BC25B-0667-4964-979C-00FBDA063795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="2145" windowWidth="15375" windowHeight="7605" activeTab="1" xr2:uid="{F05F15B4-F200-4A16-9B1F-97632D0E19C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{F05F15B4-F200-4A16-9B1F-97632D0E19C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="98">
   <si>
     <t>UserName</t>
   </si>
@@ -298,21 +298,12 @@
     <t>Trail Start Date</t>
   </si>
   <si>
-    <t>25/04/2021</t>
-  </si>
-  <si>
     <t>Physician Saved</t>
   </si>
   <si>
-    <t>25/03/2022</t>
-  </si>
-  <si>
     <t>Record Not Found</t>
   </si>
   <si>
-    <t>25/05/2021</t>
-  </si>
-  <si>
     <t>Pratip@gmail.com</t>
   </si>
   <si>
@@ -322,20 +313,22 @@
     <t>josugan2@gmail.com</t>
   </si>
   <si>
-    <t>25/06/2021</t>
-  </si>
-  <si>
     <t>mozhi2@gmail.com</t>
   </si>
   <si>
     <t>The record is not available</t>
+  </si>
+  <si>
+    <t>25/12/2021</t>
+  </si>
+  <si>
+    <t>25/12/2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -750,9 +743,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="40.140625" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="40.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -800,16 +793,16 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -837,19 +830,19 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" t="s">
         <v>89</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -857,19 +850,19 @@
         <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -880,16 +873,16 @@
         <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -897,17 +890,17 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -915,17 +908,17 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -945,9 +938,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="54.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="54" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1021,18 +1014,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="8" max="10" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="10" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="27" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="30.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1400,10 +1393,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="33.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changes in AdminLogin.java for create doctor method
</commit_message>
<xml_diff>
--- a/inputFiles/Admin_Login.xlsx
+++ b/inputFiles/Admin_Login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\EzscheulerProject\EzScheduler\inputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE78A74C-73D2-4891-89FF-74ABE0034473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D81764F-20C1-486A-B6E6-6E6DBDE1FD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{F05F15B4-F200-4A16-9B1F-97632D0E19C1}"/>
   </bookViews>
@@ -1005,7 +1005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60E0487-CC04-413F-BED3-2939739CFB5F}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes in the Doctor Tests
</commit_message>
<xml_diff>
--- a/inputFiles/Admin_Login.xlsx
+++ b/inputFiles/Admin_Login.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\EzscheulerProject\EzScheduler\inputFiles\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="100">
   <si>
     <t>UserName</t>
   </si>
@@ -320,12 +320,22 @@
   </si>
   <si>
     <t>The record is not available</t>
+  </si>
+  <si>
+    <t>Invalid email address</t>
+  </si>
+  <si>
+    <t>Please enter a Valid Mobile Number</t>
+  </si>
+  <si>
+    <t>Experience is Required</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -740,9 +750,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="40.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="40.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -795,11 +805,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -935,9 +945,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="54.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="31.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1011,18 +1021,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="10" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="27" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="10" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="30.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1110,6 +1120,9 @@
       <c r="M2" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="N2" t="s">
+        <v>42</v>
+      </c>
       <c r="O2" s="6" t="s">
         <v>42</v>
       </c>
@@ -1151,6 +1164,9 @@
       </c>
       <c r="M3" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>58</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>58</v>
@@ -1190,6 +1206,9 @@
       <c r="M4" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="N4" t="s">
+        <v>67</v>
+      </c>
       <c r="O4" s="1" t="s">
         <v>67</v>
       </c>
@@ -1230,6 +1249,9 @@
       <c r="M5" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="N5" t="s">
+        <v>97</v>
+      </c>
       <c r="O5" s="1" t="s">
         <v>69</v>
       </c>
@@ -1270,6 +1292,9 @@
       <c r="M6" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="N6" t="s">
+        <v>98</v>
+      </c>
       <c r="O6" s="1" t="s">
         <v>72</v>
       </c>
@@ -1308,6 +1333,9 @@
       <c r="M7" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="N7" t="s">
+        <v>74</v>
+      </c>
       <c r="O7" s="1" t="s">
         <v>74</v>
       </c>
@@ -1347,6 +1375,9 @@
       </c>
       <c r="M8" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="N8" t="s">
+        <v>99</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>84</v>
@@ -1369,10 +1400,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="33.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="27.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>